<commit_message>
added structure to the front end
</commit_message>
<xml_diff>
--- a/excel/repayment_schedule_Asa1.xlsx
+++ b/excel/repayment_schedule_Asa1.xlsx
@@ -384,7 +384,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -406,10 +406,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>36914</v>
+        <v>44593</v>
       </c>
       <c r="C2">
-        <v>9323.076923076924</v>
+        <v>43750</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -417,10 +417,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>36945</v>
+        <v>44621</v>
       </c>
       <c r="C3">
-        <v>9323.076923076924</v>
+        <v>43750</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -428,10 +428,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>36973</v>
+        <v>44652</v>
       </c>
       <c r="C4">
-        <v>9323.076923076924</v>
+        <v>43750</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -439,10 +439,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>37004</v>
+        <v>44682</v>
       </c>
       <c r="C5">
-        <v>9323.076923076924</v>
+        <v>43750</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -450,10 +450,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>37034</v>
+        <v>44713</v>
       </c>
       <c r="C6">
-        <v>9323.076923076924</v>
+        <v>43750</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -461,10 +461,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>37065</v>
+        <v>44743</v>
       </c>
       <c r="C7">
-        <v>9323.076923076924</v>
+        <v>43750</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -472,10 +472,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>37095</v>
+        <v>44774</v>
       </c>
       <c r="C8">
-        <v>9323.076923076924</v>
+        <v>43750</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -483,10 +483,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>37126</v>
+        <v>44805</v>
       </c>
       <c r="C9">
-        <v>9323.076923076924</v>
+        <v>43750</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -494,10 +494,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>37157</v>
+        <v>44835</v>
       </c>
       <c r="C10">
-        <v>9323.076923076924</v>
+        <v>43750</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -505,10 +505,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>37187</v>
+        <v>44866</v>
       </c>
       <c r="C11">
-        <v>9323.076923076924</v>
+        <v>43750</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -516,10 +516,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>37218</v>
+        <v>44896</v>
       </c>
       <c r="C12">
-        <v>9323.076923076924</v>
+        <v>43750</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -527,21 +527,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>37248</v>
+        <v>44927</v>
       </c>
       <c r="C13">
-        <v>9323.076923076924</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2">
-        <v>37279</v>
-      </c>
-      <c r="C14">
-        <v>9323.076923076924</v>
+        <v>43750</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code for demo fixed loan balance error
</commit_message>
<xml_diff>
--- a/excel/repayment_schedule_Asa1.xlsx
+++ b/excel/repayment_schedule_Asa1.xlsx
@@ -409,7 +409,7 @@
         <v>44593</v>
       </c>
       <c r="C2">
-        <v>1750</v>
+        <v>18333.33333333333</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -420,7 +420,7 @@
         <v>44621</v>
       </c>
       <c r="C3">
-        <v>1750</v>
+        <v>18333.33333333333</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -431,7 +431,7 @@
         <v>44652</v>
       </c>
       <c r="C4">
-        <v>1750</v>
+        <v>18333.33333333333</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -442,7 +442,7 @@
         <v>44682</v>
       </c>
       <c r="C5">
-        <v>1750</v>
+        <v>18333.33333333333</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -453,7 +453,7 @@
         <v>44713</v>
       </c>
       <c r="C6">
-        <v>1750</v>
+        <v>18333.33333333333</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -464,7 +464,7 @@
         <v>44743</v>
       </c>
       <c r="C7">
-        <v>1750</v>
+        <v>18333.33333333333</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -475,7 +475,7 @@
         <v>44774</v>
       </c>
       <c r="C8">
-        <v>1750</v>
+        <v>18333.33333333333</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -486,7 +486,7 @@
         <v>44805</v>
       </c>
       <c r="C9">
-        <v>1750</v>
+        <v>18333.33333333333</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -497,7 +497,7 @@
         <v>44835</v>
       </c>
       <c r="C10">
-        <v>1750</v>
+        <v>18333.33333333333</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -508,7 +508,7 @@
         <v>44866</v>
       </c>
       <c r="C11">
-        <v>1750</v>
+        <v>18333.33333333333</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -519,7 +519,7 @@
         <v>44896</v>
       </c>
       <c r="C12">
-        <v>1750</v>
+        <v>18333.33333333333</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -530,7 +530,7 @@
         <v>44927</v>
       </c>
       <c r="C13">
-        <v>1750</v>
+        <v>18333.33333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>